<commit_message>
Changes of name of 3 species from the start
</commit_message>
<xml_diff>
--- a/output/05.HC/clust_attribution_HC_essentials_only.xlsx
+++ b/output/05.HC/clust_attribution_HC_essentials_only.xlsx
@@ -257,7 +257,7 @@
     <t xml:space="preserve">Idiacanthus atlanticus</t>
   </si>
   <si>
-    <t xml:space="preserve">Stomias sp</t>
+    <t xml:space="preserve">Stomias spp.</t>
   </si>
   <si>
     <t xml:space="preserve">Zoarcidae</t>
@@ -2939,9 +2939,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
+      <c r="A34"/>
       <c r="B34" t="s">
         <v>79</v>
       </c>

</xml_diff>